<commit_message>
Fixed logic of Industries settings.
</commit_message>
<xml_diff>
--- a/admin/static/example.xlsx
+++ b/admin/static/example.xlsx
@@ -19,6 +19,14 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
@@ -29,6 +37,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,17 +119,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
-  </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>